<commit_message>
Added csv file with benchmark data to correct folder
</commit_message>
<xml_diff>
--- a/benchmark/CPUvsGPU.xlsx
+++ b/benchmark/CPUvsGPU.xlsx
@@ -8,13 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcinb\git-repos\WPA2Cracking\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA0B7E-00EC-438D-9CD9-4CB322F247C5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FCBB65-F2E2-4C96-8080-776430608C84}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="11366" xr2:uid="{B7BDCE11-31BA-46E8-A8E1-4BB63B3D7894}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$2:$F$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$G$2:$G$3</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$2:$D$3</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$2:$E$3</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$1</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1771,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2A8076-AA62-4D60-A8B7-D955B2218B28}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>